<commit_message>
CA agg data update
CA agg data update.  Changes to water source type and variable specific type.
</commit_message>
<xml_diff>
--- a/California/AggregatedAmounts/CA_Aggregated Schema Mapping to WaDE_QA.xlsx
+++ b/California/AggregatedAmounts/CA_Aggregated Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\California\AggregatedAmounts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36332CA7-599F-4B7D-89A7-E01597C2CF54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD20A8C-EB88-49E4-9A1A-DE79BD913728}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="645" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="645" activeTab="6" xr2:uid="{00CC2BD5-2C7C-4716-9573-3E594BB9D2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="260">
   <si>
     <t>Name</t>
   </si>
@@ -755,9 +755,6 @@
     <t xml:space="preserve">Unspecificed	</t>
   </si>
   <si>
-    <t>Groundwater, Surface Water</t>
-  </si>
-  <si>
     <t>*from shapefiles</t>
   </si>
   <si>
@@ -828,7 +825,16 @@
 CA_Depletion</t>
   </si>
   <si>
-    <t>Cutting avaible down to the follwing CategoryC fields: Applied Water Use (consumption?, Depletion (withdrawls?).</t>
+    <t>Surface and Groundwater</t>
+  </si>
+  <si>
+    <t>Cutting avaible down to the follwing CategoryC fields: Applied Water Use (consumption?) and Depletion (withdrawls?).</t>
+  </si>
+  <si>
+    <t>01/01 + Year</t>
+  </si>
+  <si>
+    <t>12/31 + Year</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1537,6 +1543,9 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1854,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE91C3C-F676-4E77-8227-802554E4B42D}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2443,7 +2452,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="34"/>
@@ -2667,7 +2676,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="96"/>
@@ -2695,7 +2704,7 @@
         <v>15</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F13" s="26"/>
       <c r="G13" s="96"/>
@@ -3107,7 +3116,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3402,7 +3411,7 @@
         <v>15</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>238</v>
+        <v>256</v>
       </c>
       <c r="F10" s="86" t="s">
         <v>11</v>
@@ -3445,7 +3454,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3604,10 +3613,10 @@
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="21" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="94" t="s">
@@ -3634,13 +3643,13 @@
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G7" s="110" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H7" s="94" t="s">
         <v>11</v>
@@ -3666,13 +3675,13 @@
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G8" s="110" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H8" s="94" t="s">
         <v>11</v>
@@ -3726,7 +3735,7 @@
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -3894,8 +3903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E07544-54C6-4298-B1F4-AA27E9BE2694}">
   <dimension ref="A1:K16431"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4180,7 +4189,7 @@
         <v>11</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G11" s="39"/>
       <c r="H11" s="16" t="s">
@@ -4207,7 +4216,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="105" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="39"/>
@@ -4236,7 +4245,7 @@
         <v>11</v>
       </c>
       <c r="E13" s="47" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="48"/>
@@ -4294,13 +4303,13 @@
         <v>11</v>
       </c>
       <c r="E15" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="G15" s="49" t="s">
         <v>249</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>244</v>
-      </c>
-      <c r="G15" s="49" t="s">
-        <v>250</v>
       </c>
       <c r="H15" s="16" t="s">
         <v>11</v>
@@ -4326,13 +4335,13 @@
         <v>15</v>
       </c>
       <c r="E16" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="G16" s="25" t="s">
         <v>251</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>244</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>252</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="27" t="s">
@@ -4770,10 +4779,10 @@
         <v>15</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G30" s="25" t="s">
         <v>134</v>
@@ -4833,14 +4842,14 @@
       <c r="D32" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="24" t="s">
-        <v>225</v>
+      <c r="E32" s="111" t="s">
+        <v>259</v>
       </c>
       <c r="F32" s="24" t="s">
         <v>11</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>11</v>
+        <v>134</v>
       </c>
       <c r="H32" s="16" t="s">
         <v>11</v>
@@ -4865,14 +4874,14 @@
       <c r="D33" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="24" t="s">
-        <v>225</v>
+      <c r="E33" s="111" t="s">
+        <v>258</v>
       </c>
       <c r="F33" s="24" t="s">
         <v>11</v>
       </c>
       <c r="G33" s="25" t="s">
-        <v>11</v>
+        <v>134</v>
       </c>
       <c r="H33" s="16" t="s">
         <v>11</v>

</xml_diff>